<commit_message>
AG/HW: Updates for v2 of the remote monitoring solution accelerator
</commit_message>
<xml_diff>
--- a/HOL/IOTHubPiHackathon/IoTHOL-LabParameters.xlsx
+++ b/HOL/IOTHubPiHackathon/IoTHOL-LabParameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinhong\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hawilkin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04A1D01A-74F4-4DFC-B37F-EAFDC15BBF4C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="12353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>IoT Hands on Lab Configuration Parameters Reference Doc</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve">   IoT Hub hostname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Device key</t>
   </si>
   <si>
     <t xml:space="preserve">   Pi Password</t>
@@ -62,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,103 +440,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="4"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="4"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>